<commit_message>
Mouse buttons, weapon ranges/atk, database
Mouse handler supports left, middle, right clicks
Fixed database error with Javelin range "1~1" -> "1~2"
Unit attack and ranges now determined by weapon
button and bar lists changed to HashMaps for functionality improvement
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computer\Documents\NetBeansProjects\GridGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -619,11 +619,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -1308,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>0</v>

</xml_diff>